<commit_message>
Nomina Dic 16 - 24
Se suben los reportes de la nomina
</commit_message>
<xml_diff>
--- a/3. Resultados/04. resultados DIC 16 al DIC 24/0. Consolidado.xlsx
+++ b/3. Resultados/04. resultados DIC 16 al DIC 24/0. Consolidado.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M295"/>
+  <dimension ref="A1:M298"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -14554,7 +14554,7 @@
     <row r="280">
       <c r="B280" t="inlineStr">
         <is>
-          <t>30/12/2024</t>
+          <t>24/12/2024</t>
         </is>
       </c>
       <c r="D280" t="inlineStr">
@@ -14998,7 +14998,7 @@
     <row r="292">
       <c r="B292" t="inlineStr">
         <is>
-          <t>30/12/2024</t>
+          <t>10/01/2025</t>
         </is>
       </c>
       <c r="D292" t="inlineStr">
@@ -15033,146 +15033,257 @@
       </c>
     </row>
     <row r="293">
-      <c r="A293">
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>24/12/2024</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>Descuento - Anticipo</t>
+        </is>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>Ivonne Mancipe</t>
+        </is>
+      </c>
+      <c r="G293" t="inlineStr">
+        <is>
+          <t>Descuento</t>
+        </is>
+      </c>
+      <c r="H293">
+        <v>0</v>
+      </c>
+      <c r="I293">
+        <v>0</v>
+      </c>
+      <c r="J293">
+        <v>0</v>
+      </c>
+      <c r="K293">
+        <v>0</v>
+      </c>
+      <c r="L293">
+        <v>-20000</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>24/12/2024</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>Descuento - Anticipo</t>
+        </is>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>Ivonne Mancipe</t>
+        </is>
+      </c>
+      <c r="G294" t="inlineStr">
+        <is>
+          <t>Descuento</t>
+        </is>
+      </c>
+      <c r="H294">
+        <v>0</v>
+      </c>
+      <c r="I294">
+        <v>0</v>
+      </c>
+      <c r="J294">
+        <v>0</v>
+      </c>
+      <c r="K294">
+        <v>0</v>
+      </c>
+      <c r="L294">
+        <v>-200000</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>24/12/2024</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>Descuento - 4 Aluerzos</t>
+        </is>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>Ivonne Mancipe</t>
+        </is>
+      </c>
+      <c r="G295" t="inlineStr">
+        <is>
+          <t>Descuento</t>
+        </is>
+      </c>
+      <c r="H295">
+        <v>0</v>
+      </c>
+      <c r="I295">
+        <v>0</v>
+      </c>
+      <c r="J295">
+        <v>0</v>
+      </c>
+      <c r="K295">
+        <v>0</v>
+      </c>
+      <c r="L295">
+        <v>-60000</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296">
         <v>36276761</v>
       </c>
-      <c r="B293" t="inlineStr">
+      <c r="B296" t="inlineStr">
         <is>
           <t>21/12/2024 13:34</t>
         </is>
       </c>
-      <c r="C293" t="inlineStr">
+      <c r="C296" t="inlineStr">
         <is>
           <t>Diana Reina (Pago Anticipado)</t>
         </is>
       </c>
-      <c r="D293" t="inlineStr">
+      <c r="D296" t="inlineStr">
         <is>
           <t>Masaje Relajante Espalda</t>
         </is>
       </c>
-      <c r="E293" t="inlineStr">
+      <c r="E296" t="inlineStr">
         <is>
           <t>Nydia Gamba</t>
         </is>
       </c>
-      <c r="F293">
-        <v>0</v>
-      </c>
-      <c r="G293" t="inlineStr">
+      <c r="F296">
+        <v>0</v>
+      </c>
+      <c r="G296" t="inlineStr">
         <is>
           <t>Ajuste</t>
         </is>
       </c>
-      <c r="H293">
-        <v>0</v>
-      </c>
-      <c r="I293">
-        <v>0</v>
-      </c>
-      <c r="J293">
-        <v>0</v>
-      </c>
-      <c r="K293">
-        <v>0</v>
-      </c>
-      <c r="L293">
+      <c r="H296">
+        <v>0</v>
+      </c>
+      <c r="I296">
+        <v>0</v>
+      </c>
+      <c r="J296">
+        <v>0</v>
+      </c>
+      <c r="K296">
+        <v>0</v>
+      </c>
+      <c r="L296">
         <v>-80000</v>
       </c>
     </row>
-    <row r="294">
-      <c r="A294">
+    <row r="297">
+      <c r="A297">
         <v>36226123</v>
       </c>
-      <c r="B294" t="inlineStr">
+      <c r="B297" t="inlineStr">
         <is>
           <t>20/12/2024 15:34</t>
         </is>
       </c>
-      <c r="C294" t="inlineStr">
+      <c r="C297" t="inlineStr">
         <is>
           <t>Karen Nieto (Pago Anticipado)</t>
         </is>
       </c>
-      <c r="D294" t="inlineStr">
+      <c r="D297" t="inlineStr">
         <is>
           <t>depilacion cejas y bigote (hilo)</t>
         </is>
       </c>
-      <c r="E294" t="inlineStr">
+      <c r="E297" t="inlineStr">
         <is>
           <t>Nydia Gamba</t>
         </is>
       </c>
-      <c r="F294">
-        <v>0</v>
-      </c>
-      <c r="G294" t="inlineStr">
+      <c r="F297">
+        <v>0</v>
+      </c>
+      <c r="G297" t="inlineStr">
         <is>
           <t>Ajuste</t>
         </is>
       </c>
-      <c r="H294">
-        <v>0</v>
-      </c>
-      <c r="I294">
-        <v>0</v>
-      </c>
-      <c r="J294">
-        <v>0</v>
-      </c>
-      <c r="K294">
-        <v>0</v>
-      </c>
-      <c r="L294">
+      <c r="H297">
+        <v>0</v>
+      </c>
+      <c r="I297">
+        <v>0</v>
+      </c>
+      <c r="J297">
+        <v>0</v>
+      </c>
+      <c r="K297">
+        <v>0</v>
+      </c>
+      <c r="L297">
         <v>-43000</v>
       </c>
     </row>
-    <row r="295">
-      <c r="A295">
+    <row r="298">
+      <c r="A298">
         <v>36190098</v>
       </c>
-      <c r="B295" t="inlineStr">
+      <c r="B298" t="inlineStr">
         <is>
           <t>19/12/2024 20:40</t>
         </is>
       </c>
-      <c r="C295" t="inlineStr">
+      <c r="C298" t="inlineStr">
         <is>
           <t>Rosanidia Peña (Pago Anticipado)</t>
         </is>
       </c>
-      <c r="D295" t="inlineStr">
+      <c r="D298" t="inlineStr">
         <is>
           <t>Pestañas set express seda</t>
         </is>
       </c>
-      <c r="E295" t="inlineStr">
+      <c r="E298" t="inlineStr">
         <is>
           <t>Nydia Gamba</t>
         </is>
       </c>
-      <c r="F295">
-        <v>0</v>
-      </c>
-      <c r="G295" t="inlineStr">
+      <c r="F298">
+        <v>0</v>
+      </c>
+      <c r="G298" t="inlineStr">
         <is>
           <t>Ajuste</t>
         </is>
       </c>
-      <c r="H295">
-        <v>0</v>
-      </c>
-      <c r="I295">
-        <v>0</v>
-      </c>
-      <c r="J295">
-        <v>0</v>
-      </c>
-      <c r="K295">
-        <v>0</v>
-      </c>
-      <c r="L295">
+      <c r="H298">
+        <v>0</v>
+      </c>
+      <c r="I298">
+        <v>0</v>
+      </c>
+      <c r="J298">
+        <v>0</v>
+      </c>
+      <c r="K298">
+        <v>0</v>
+      </c>
+      <c r="L298">
         <v>-100000</v>
       </c>
     </row>

</xml_diff>